<commit_message>
Update num.txt | 2024-10-09 08:11:24 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
   <si>
     <t>回数</t>
   </si>
@@ -34,6 +34,27 @@
     <t>開催案内</t>
   </si>
   <si>
+    <t>第596回</t>
+  </si>
+  <si>
+    <t>2024年10月9日（令和6年10月9日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
+２臨床検査の保険適用について
+３歯科用貴金属価格の随時改定について
+４第25回医療経済実態調査について
+５ＤＰＣ合併・退出等審査会における審査結果及び今後の対応について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
+  </si>
+  <si>
     <t>第595回</t>
   </si>
   <si>
@@ -41,13 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">１高額医薬品（認知症薬）に対する対応について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -69,6 +83,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">議事録
+</t>
+  </si>
+  <si>
     <t>第593回</t>
   </si>
   <si>
@@ -82,10 +100,6 @@
 ５DPC における高額な新規の医薬品等への対応について
 ６放射性医薬品を用いたPET 検査の取扱い変更に伴う掲示事項等告示の 一部改正について
 ７その他（再生医療等製品）
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -747,7 +761,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -924,7 +938,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -944,7 +958,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1290,6 +1304,26 @@
         <v>10</v>
       </c>
       <c r="F27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Update num.txt | 2024-10-09 08:11:24 JST"
This reverts commit f1b3d96fd7629e855e8710074d1603e2a59fb29c.
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
   <si>
     <t>回数</t>
   </si>
@@ -34,17 +34,13 @@
     <t>開催案内</t>
   </si>
   <si>
-    <t>第596回</t>
-  </si>
-  <si>
-    <t>2024年10月9日（令和6年10月9日）</t>
-  </si>
-  <si>
-    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
-２臨床検査の保険適用について
-３歯科用貴金属価格の随時改定について
-４第25回医療経済実態調査について
-５ＤＰＣ合併・退出等審査会における審査結果及び今後の対応について
+    <t>第595回</t>
+  </si>
+  <si>
+    <t>2024年9月25日（令和6年9月25日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１高額医薬品（認知症薬）に対する対応について
 </t>
   </si>
   <si>
@@ -52,16 +48,6 @@
   </si>
   <si>
     <t xml:space="preserve">資料
-</t>
-  </si>
-  <si>
-    <t>第595回</t>
-  </si>
-  <si>
-    <t>2024年9月25日（令和6年9月25日）</t>
-  </si>
-  <si>
-    <t xml:space="preserve">１高額医薬品（認知症薬）に対する対応について
 </t>
   </si>
   <si>
@@ -83,10 +69,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">議事録
-</t>
-  </si>
-  <si>
     <t>第593回</t>
   </si>
   <si>
@@ -100,6 +82,10 @@
 ５DPC における高額な新規の医薬品等への対応について
 ６放射性医薬品を用いたPET 検査の取扱い変更に伴う掲示事項等告示の 一部改正について
 ７その他（再生医療等製品）
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -761,7 +747,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -938,7 +924,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -958,7 +944,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1304,26 +1290,6 @@
         <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2024-10-12 14:25:56 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
   <si>
     <t>回数</t>
   </si>
@@ -34,6 +34,27 @@
     <t>開催案内</t>
   </si>
   <si>
+    <t>第596回</t>
+  </si>
+  <si>
+    <t>2024年10月9日（令和6年10月9日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
+２臨床検査の保険適用について
+３歯科用貴金属価格の随時改定について
+４第25回医療経済実態調査について
+５ＤＰＣ合併・退出等審査会における審査結果及び今後の対応について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
+  </si>
+  <si>
     <t>第595回</t>
   </si>
   <si>
@@ -44,10 +65,7 @@
 </t>
   </si>
   <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -82,10 +100,6 @@
 ５DPC における高額な新規の医薬品等への対応について
 ６放射性医薬品を用いたPET 検査の取扱い変更に伴う掲示事項等告示の 一部改正について
 ７その他（再生医療等製品）
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -747,7 +761,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -804,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -815,16 +829,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -844,7 +858,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -864,7 +878,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -884,7 +898,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -904,7 +918,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -924,7 +938,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -944,7 +958,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -964,7 +978,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -984,7 +998,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1004,7 +1018,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1024,7 +1038,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1044,7 +1058,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1064,7 +1078,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1084,7 +1098,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1104,7 +1118,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1124,7 +1138,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1144,7 +1158,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1164,7 +1178,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1184,7 +1198,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1204,7 +1218,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1224,7 +1238,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1244,7 +1258,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1264,7 +1278,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1284,12 +1298,32 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
       </c>
       <c r="F27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Update num.txt | 2024-10-12 14:25:56 JST"
This reverts commit 090fb34f8a506837da67b44a34c6a8de5590c467.
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
   <si>
     <t>回数</t>
   </si>
@@ -34,17 +34,13 @@
     <t>開催案内</t>
   </si>
   <si>
-    <t>第596回</t>
-  </si>
-  <si>
-    <t>2024年10月9日（令和6年10月9日）</t>
-  </si>
-  <si>
-    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
-２臨床検査の保険適用について
-３歯科用貴金属価格の随時改定について
-４第25回医療経済実態調査について
-５ＤＰＣ合併・退出等審査会における審査結果及び今後の対応について
+    <t>第595回</t>
+  </si>
+  <si>
+    <t>2024年9月25日（令和6年9月25日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１高額医薬品（認知症薬）に対する対応について
 </t>
   </si>
   <si>
@@ -52,20 +48,6 @@
   </si>
   <si>
     <t xml:space="preserve">資料
-</t>
-  </si>
-  <si>
-    <t>第595回</t>
-  </si>
-  <si>
-    <t>2024年9月25日（令和6年9月25日）</t>
-  </si>
-  <si>
-    <t xml:space="preserve">１高額医薬品（認知症薬）に対する対応について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -100,6 +82,10 @@
 ５DPC における高額な新規の医薬品等への対応について
 ６放射性医薬品を用いたPET 検査の取扱い変更に伴う掲示事項等告示の 一部改正について
 ７その他（再生医療等製品）
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -761,7 +747,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -818,7 +804,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -829,16 +815,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -858,7 +844,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -878,7 +864,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -898,7 +884,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -918,7 +904,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -938,7 +924,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -958,7 +944,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -978,7 +964,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -998,7 +984,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1018,7 +1004,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1038,7 +1024,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1058,7 +1044,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1078,7 +1064,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1098,7 +1084,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1118,7 +1104,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1138,7 +1124,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1158,7 +1144,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1178,7 +1164,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1198,7 +1184,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1218,7 +1204,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1238,7 +1224,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1258,7 +1244,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1278,7 +1264,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1298,32 +1284,12 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2024-10-13 08:10:02 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
   <si>
     <t>回数</t>
   </si>
@@ -34,6 +34,27 @@
     <t>開催案内</t>
   </si>
   <si>
+    <t>第596回</t>
+  </si>
+  <si>
+    <t>2024年10月9日（令和6年10月9日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
+２臨床検査の保険適用について
+３歯科用貴金属価格の随時改定について
+４第25回医療経済実態調査について
+５ＤＰＣ合併・退出等審査会における審査結果及び今後の対応について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
+  </si>
+  <si>
     <t>第595回</t>
   </si>
   <si>
@@ -44,10 +65,7 @@
 </t>
   </si>
   <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -82,10 +100,6 @@
 ５DPC における高額な新規の医薬品等への対応について
 ６放射性医薬品を用いたPET 検査の取扱い変更に伴う掲示事項等告示の 一部改正について
 ７その他（再生医療等製品）
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -747,7 +761,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -804,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -815,16 +829,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -844,7 +858,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -864,7 +878,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -884,7 +898,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -904,7 +918,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -924,7 +938,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -944,7 +958,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -964,7 +978,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -984,7 +998,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1004,7 +1018,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1024,7 +1038,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1044,7 +1058,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1064,7 +1078,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1084,7 +1098,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1104,7 +1118,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1124,7 +1138,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1144,7 +1158,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1164,7 +1178,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1184,7 +1198,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1204,7 +1218,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1224,7 +1238,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1244,7 +1258,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1264,7 +1278,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1284,12 +1298,32 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
       </c>
       <c r="F27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2024-11-06 08:10:37 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="93">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,26 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第597回</t>
+  </si>
+  <si>
+    <t>2024年11月6日（令和6年11月6日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１診療報酬基本問題小委員会からの報告について
+２令和６年能登半島地震による被災地特例措置の今後の取り扱いについて(案)
+３ＤＰＣ対象病院の合併・退出等にかかる手続きの見直しについて
+４マイナ保険証の利用促進等について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第596回</t>
@@ -48,10 +68,7 @@
 </t>
   </si>
   <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -62,10 +79,6 @@
   </si>
   <si>
     <t xml:space="preserve">１高額医薬品（認知症薬）に対する対応について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -761,7 +774,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -958,7 +971,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -978,7 +991,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1324,6 +1337,26 @@
         <v>10</v>
       </c>
       <c r="F28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2024-11-13 08:10:49 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,32 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第598回</t>
+  </si>
+  <si>
+    <t>2024年11月13日（令和6年11月13日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１高額医薬品（認知症薬）に対する対応について
+２医薬品の新規薬価収載等について
+３最適使用推進ガイドラインについて
+４費用対効果評価の結果を踏まえた薬価の見直しについて
+５医療機器、臨床検査及び PET の保険適用について
+６診療報酬改定結果検証部会からの報告について
+７ＤＰＣにおける高額な新規の医薬品等への対応について
+８在宅自己注射について
+９保険医療機関等における資格確認方法の変更に伴う所要の見直しについて（諮問）
+10個別改定項目について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第597回</t>
@@ -44,13 +70,6 @@
 ２令和６年能登半島地震による被災地特例措置の今後の取り扱いについて(案)
 ３ＤＰＣ対象病院の合併・退出等にかかる手続きの見直しについて
 ４マイナ保険証の利用促進等について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -774,7 +793,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -831,7 +850,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -842,16 +861,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -871,7 +890,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -891,7 +910,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -911,7 +930,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -931,7 +950,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -951,7 +970,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -971,7 +990,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -991,7 +1010,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1011,7 +1030,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1031,7 +1050,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1051,7 +1070,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1071,7 +1090,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1091,7 +1110,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1111,7 +1130,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1131,7 +1150,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1151,7 +1170,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1171,7 +1190,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1191,7 +1210,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1211,7 +1230,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1231,7 +1250,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1251,7 +1270,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1271,7 +1290,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1291,7 +1310,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1311,7 +1330,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1331,7 +1350,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1351,12 +1370,32 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
       </c>
       <c r="F29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2024-12-11 08:11:05 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="99">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第599回</t>
+  </si>
+  <si>
+    <t>2024年12月11日（令和6年12月11日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
+２最適使用推進ガイドラインについて（報告）
+３先進医療会議からの報告について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第598回</t>
@@ -50,13 +69,11 @@
 ８在宅自己注射について
 ９保険医療機関等における資格確認方法の変更に伴う所要の見直しについて（諮問）
 10個別改定項目について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
+11答申について
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -84,10 +101,6 @@
 ３歯科用貴金属価格の随時改定について
 ４第25回医療経済実態調査について
 ５ＤＰＣ合併・退出等審査会における審査結果及び今後の対応について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -793,7 +806,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -850,7 +863,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -861,16 +874,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -890,7 +903,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -910,7 +923,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -930,7 +943,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -950,7 +963,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -970,7 +983,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -990,7 +1003,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1010,7 +1023,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1030,7 +1043,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1050,7 +1063,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1070,7 +1083,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1090,7 +1103,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1110,7 +1123,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1130,7 +1143,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1150,7 +1163,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1170,7 +1183,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1190,7 +1203,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1210,7 +1223,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1230,7 +1243,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1250,7 +1263,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1270,7 +1283,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1290,7 +1303,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1310,7 +1323,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1330,7 +1343,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1350,7 +1363,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1370,7 +1383,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1390,12 +1403,32 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
       </c>
       <c r="F30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2024-12-18 08:10:48 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="102">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第600回</t>
+  </si>
+  <si>
+    <t>2024年12月18日（令和6年12月18日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１調査実施小委員会からの報告について
+２ＤＰＣ対象病院の退出に係る報告について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第599回</t>
@@ -43,13 +61,6 @@
     <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
 ２最適使用推進ガイドラインについて（報告）
 ３先進医療会議からの報告について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -806,7 +817,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -863,7 +874,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -874,16 +885,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -903,7 +914,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -923,7 +934,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -943,7 +954,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -963,7 +974,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -983,7 +994,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1003,7 +1014,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1023,7 +1034,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1043,7 +1054,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1063,7 +1074,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1083,7 +1094,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1103,7 +1114,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1123,7 +1134,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1143,7 +1154,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1163,7 +1174,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1183,7 +1194,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1203,7 +1214,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1223,7 +1234,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1243,7 +1254,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1263,7 +1274,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1283,7 +1294,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1303,7 +1314,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1323,7 +1334,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1343,7 +1354,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1363,7 +1374,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1383,7 +1394,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1403,7 +1414,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1423,12 +1434,32 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
       </c>
       <c r="F31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2024-12-26 08:10:18 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="105">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第601回</t>
+  </si>
+  <si>
+    <t>2024年12月25日（令和6年12月25日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１令和７年度薬価改定の骨子（案）について
+２DPC/PDPS における令和６年能登半島地震等を踏まえた対応について
+３中間年改定の年に行う期中の診療報酬改定について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第600回</t>
@@ -42,13 +61,6 @@
   <si>
     <t xml:space="preserve">１調査実施小委員会からの報告について
 ２ＤＰＣ対象病院の退出に係る報告について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -817,7 +829,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -894,7 +906,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -905,16 +917,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -934,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -954,7 +966,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -974,7 +986,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -994,7 +1006,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1014,7 +1026,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1034,7 +1046,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1054,7 +1066,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1074,7 +1086,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1094,7 +1106,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1114,7 +1126,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1134,7 +1146,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1154,7 +1166,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1174,7 +1186,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1194,7 +1206,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1214,7 +1226,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1234,7 +1246,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1254,7 +1266,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1274,7 +1286,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1294,7 +1306,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1314,7 +1326,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1334,7 +1346,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1354,7 +1366,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1374,7 +1386,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1394,7 +1406,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1414,7 +1426,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1434,7 +1446,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1454,12 +1466,32 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
       </c>
       <c r="F32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-01-15 08:10:01 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="108">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,27 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第602回</t>
+  </si>
+  <si>
+    <t>2025年1月15日（令和7年1月15日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１医療機器の保険適用について
+２令和７年度薬価改定について
+３改定時加算について
+４歯科用貴金属価格の随時改定について
+５中間年改定の年に行う期中の診療報酬改定について（諮問）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第601回</t>
@@ -43,13 +64,6 @@
     <t xml:space="preserve">１令和７年度薬価改定の骨子（案）について
 ２DPC/PDPS における令和６年能登半島地震等を踏まえた対応について
 ３中間年改定の年に行う期中の診療報酬改定について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -829,7 +843,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -926,7 +940,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -937,16 +951,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -966,7 +980,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -986,7 +1000,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1006,7 +1020,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1026,7 +1040,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1046,7 +1060,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1066,7 +1080,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1086,7 +1100,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1106,7 +1120,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1126,7 +1140,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1146,7 +1160,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1166,7 +1180,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1186,7 +1200,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1206,7 +1220,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1226,7 +1240,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1246,7 +1260,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1266,7 +1280,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1286,7 +1300,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1306,7 +1320,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1326,7 +1340,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1346,7 +1360,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1366,7 +1380,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1386,7 +1400,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1406,7 +1420,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1426,7 +1440,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1446,7 +1460,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1466,7 +1480,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1486,12 +1500,32 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
       </c>
       <c r="F33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-01-29 08:10:06 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="111">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,28 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第603回</t>
+  </si>
+  <si>
+    <t>2025年1月29日（令和7年1月29日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
+２先進医療会議及び患者申出療養評価会議からの報告について_x000D_
+３DPC 対象病院の再編に係る報告について
+４その他
+５医療 DX に係る診療報酬上の評価の取扱いについて（諮問）
+６個別改定項目について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第602回</t>
@@ -48,13 +70,6 @@
 </t>
   </si>
   <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
-</t>
-  </si>
-  <si>
     <t>第601回</t>
   </si>
   <si>
@@ -64,6 +79,10 @@
     <t xml:space="preserve">１令和７年度薬価改定の骨子（案）について
 ２DPC/PDPS における令和６年能登半島地震等を踏まえた対応について
 ３中間年改定の年に行う期中の診療報酬改定について
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -107,10 +126,6 @@
 ９保険医療機関等における資格確認方法の変更に伴う所要の見直しについて（諮問）
 10個別改定項目について
 11答申について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -843,7 +858,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -920,7 +935,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -931,16 +946,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -951,16 +966,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -980,7 +995,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1000,7 +1015,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1020,7 +1035,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1040,7 +1055,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1060,7 +1075,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1080,7 +1095,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1100,7 +1115,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1120,7 +1135,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1140,7 +1155,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1160,7 +1175,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1180,7 +1195,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1200,7 +1215,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1220,7 +1235,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1240,7 +1255,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1260,7 +1275,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1280,7 +1295,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1300,7 +1315,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1320,7 +1335,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1340,7 +1355,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1360,7 +1375,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1380,7 +1395,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1400,7 +1415,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1420,7 +1435,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1440,7 +1455,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1460,7 +1475,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1480,7 +1495,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1500,7 +1515,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1520,12 +1535,32 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
       </c>
       <c r="F34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-02-19 08:10:37 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="114">
   <si>
     <t>回数</t>
   </si>
@@ -34,6 +34,26 @@
     <t>開催案内</t>
   </si>
   <si>
+    <t>第604回</t>
+  </si>
+  <si>
+    <t>2025年2月19日（令和7年2月19日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
+２「造血器腫瘍又は類縁疾患ゲノムプロファイリング検査」のＤＰＣ制度 における取扱いについて
+３薬価算定の基準の改正について
+４診療報酬基本問題小委員会からの報告について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
+  </si>
+  <si>
     <t>第603回</t>
   </si>
   <si>
@@ -41,18 +61,13 @@
   </si>
   <si>
     <t xml:space="preserve">１費用対効果評価専門組織からの報告について
-２先進医療会議及び患者申出療養評価会議からの報告について_x000D_
+２先進医療会議及び患者申出療養評価会議からの報告について
 ３DPC 対象病院の再編に係る報告について
 ４その他
 ５医療 DX に係る診療報酬上の評価の取扱いについて（諮問）
 ６個別改定項目について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
+７答申書附帯意見について
+８答申について
 </t>
   </si>
   <si>
@@ -70,6 +85,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">議事録
+</t>
+  </si>
+  <si>
     <t>第601回</t>
   </si>
   <si>
@@ -79,10 +98,6 @@
     <t xml:space="preserve">１令和７年度薬価改定の骨子（案）について
 ２DPC/PDPS における令和６年能登半島地震等を踏まえた対応について
 ３中間年改定の年に行う期中の診療報酬改定について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -858,7 +873,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1195,7 +1210,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1215,7 +1230,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1561,6 +1576,26 @@
         <v>10</v>
       </c>
       <c r="F35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-03-12 08:10:53 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="117">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,35 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第605回</t>
+  </si>
+  <si>
+    <t>2025年3月12日（令和7年3月12日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１医療機器の保険適用について
+２医薬品の新規薬価収載について
+３最適使用推進ガイドラインについて(審議)
+４DPC における高額な新規の医薬品等への対応について
+５在宅自己注射について
+６最適使用推進ガイドラインについて（報告）
+７費用対効果評価の結果による材料価格及び薬価の価格調整について
+８公知申請とされた適応外薬の保険適用について
+９先進医療会議からの報告について
+10令和６年能登半島地震による被災に伴う被災地特例措置の今後の取扱いについて(案)
+11ＤＰＣ対象病院の再編及び退出に係る報告について
+12訪問看護ステーションの指導監査について
+13薬機法等一部改正法案の概要（安定供給関係）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第604回</t>
@@ -44,13 +73,6 @@
 ２「造血器腫瘍又は類縁疾患ゲノムプロファイリング検査」のＤＰＣ制度 における取扱いについて
 ３薬価算定の基準の改正について
 ４診療報酬基本問題小委員会からの報告について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -71,6 +93,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">議事録
+</t>
+  </si>
+  <si>
     <t>第602回</t>
   </si>
   <si>
@@ -82,10 +108,6 @@
 ３改定時加算について
 ４歯科用貴金属価格の随時改定について
 ５中間年改定の年に行う期中の診療報酬改定について（諮問）
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -873,7 +895,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1230,7 +1252,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1250,7 +1272,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1596,6 +1618,26 @@
         <v>10</v>
       </c>
       <c r="F36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-04-09 08:11:18 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="120">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,30 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第606回</t>
+  </si>
+  <si>
+    <t>2025年4月9日（令和7年4月9日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１部会・小委員会に属する委員の指名等について
+２医療機器の保険適用について
+３医薬品の新規薬価収載について
+４DPC における高額な新規の医薬品等への対応について
+５在宅自己注射について
+６DPC 対象病院の退出に係る報告について
+７令和８年度診療報酬改定、薬価改定の議論の進め方について
+８選定療養に導入すべき事例等に関する提案・意見募集について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第605回</t>
@@ -56,10 +80,7 @@
 </t>
   </si>
   <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -90,10 +111,6 @@
 ６個別改定項目について
 ７答申書附帯意見について
 ８答申について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -895,7 +912,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -952,7 +969,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -963,16 +980,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -992,7 +1009,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1012,7 +1029,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1032,7 +1049,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1052,7 +1069,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1072,7 +1089,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1092,7 +1109,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1112,7 +1129,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1132,7 +1149,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1152,7 +1169,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1172,7 +1189,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1192,7 +1209,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1212,7 +1229,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1232,7 +1249,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1252,7 +1269,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1272,7 +1289,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1292,7 +1309,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1312,7 +1329,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1332,7 +1349,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1352,7 +1369,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1372,7 +1389,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1392,7 +1409,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1412,7 +1429,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1432,7 +1449,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1452,7 +1469,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1472,7 +1489,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1492,7 +1509,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1512,7 +1529,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1532,7 +1549,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1552,7 +1569,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1572,7 +1589,7 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1592,7 +1609,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1612,7 +1629,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1632,12 +1649,32 @@
         <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
       </c>
       <c r="F37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-04-23 08:11:23 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="123">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,27 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第607回</t>
+  </si>
+  <si>
+    <t>2025年4月23日（令和7年4月23日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
+２入院・外来医療等の調査・評価分科会からの報告について
+３歯科用貴金属価格の随時改定について
+４診療報酬改定結果検証部会からの報告について
+５医療機関を取り巻く状況について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第606回</t>
@@ -48,13 +69,6 @@
 ６DPC 対象病院の退出に係る報告について
 ７令和８年度診療報酬改定、薬価改定の議論の進め方について
 ８選定療養に導入すべき事例等に関する提案・意見募集について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -912,7 +926,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -969,7 +983,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -980,16 +994,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1009,7 +1023,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1029,7 +1043,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1049,7 +1063,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1069,7 +1083,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1089,7 +1103,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1109,7 +1123,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1129,7 +1143,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1149,7 +1163,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1169,7 +1183,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1189,7 +1203,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1209,7 +1223,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1229,7 +1243,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1249,7 +1263,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1269,7 +1283,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1289,7 +1303,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1309,7 +1323,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1329,7 +1343,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1349,7 +1363,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1369,7 +1383,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1389,7 +1403,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1409,7 +1423,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1429,7 +1443,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1449,7 +1463,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1469,7 +1483,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1489,7 +1503,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1509,7 +1523,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1529,7 +1543,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1549,7 +1563,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1569,7 +1583,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1589,7 +1603,7 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1609,7 +1623,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1629,7 +1643,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1649,7 +1663,7 @@
         <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1669,12 +1683,32 @@
         <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
       </c>
       <c r="F38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-05-14 08:11:55 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="126">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,31 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第608回</t>
+  </si>
+  <si>
+    <t>2025年5月14日（令和7年5月14日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
+２医療機器及び臨床検査の保険適用について
+３医薬品の新規薬価収載等について
+４最適使用推進ガイドラインについて
+５費用対効果評価の結果を踏まえた薬価の見直しについて
+６条件及び期限付き承認を受けた再生医療等製品の保険適用について
+７DPC における高額な新規の医薬品等への対応について
+８在宅自己注射について
+９令和７年度における DPC/PDPS の現況について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第607回</t>
@@ -45,13 +70,6 @@
 ３歯科用貴金属価格の随時改定について
 ４診療報酬改定結果検証部会からの報告について
 ５医療機関を取り巻く状況について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -69,6 +87,10 @@
 ６DPC 対象病院の退出に係る報告について
 ７令和８年度診療報酬改定、薬価改定の議論の進め方について
 ８選定療養に導入すべき事例等に関する提案・意見募集について
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -91,10 +113,6 @@
 11ＤＰＣ対象病院の再編及び退出に係る報告について
 12訪問看護ステーションの指導監査について
 13薬機法等一部改正法案の概要（安定供給関係）
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -926,7 +944,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1343,7 +1361,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1363,7 +1381,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1709,6 +1727,26 @@
         <v>10</v>
       </c>
       <c r="F39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-06-18 08:12:12 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="129">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,30 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第609回</t>
+  </si>
+  <si>
+    <t>2025年6月18日（令和7年6月18日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１部会・小委員会に属する委員の指名等について
+２再生医療等製品の医療保険上の取扱いについて
+３入院・外来医療等の調査・評価分科会からの報告について
+４医療機器の保険適用について
+５先進医療会議からの報告について
+６最適使用推進ガイドラインについて(報告)
+７公知申請とされた適応外薬の保険適用について
+８薬価基準から削除する品目について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第608回</t>
@@ -52,10 +76,7 @@
 </t>
   </si>
   <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -87,10 +108,6 @@
 ６DPC 対象病院の退出に係る報告について
 ７令和８年度診療報酬改定、薬価改定の議論の進め方について
 ８選定療養に導入すべき事例等に関する提案・意見募集について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -944,7 +961,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1001,7 +1018,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -1012,16 +1029,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1041,7 +1058,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1061,7 +1078,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1081,7 +1098,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1101,7 +1118,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1121,7 +1138,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1141,7 +1158,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1161,7 +1178,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1181,7 +1198,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1201,7 +1218,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1221,7 +1238,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1241,7 +1258,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1261,7 +1278,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1281,7 +1298,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1301,7 +1318,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1321,7 +1338,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1341,7 +1358,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1361,7 +1378,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1381,7 +1398,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1401,7 +1418,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1421,7 +1438,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1441,7 +1458,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1461,7 +1478,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1481,7 +1498,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1501,7 +1518,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1521,7 +1538,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1541,7 +1558,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1561,7 +1578,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1581,7 +1598,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1601,7 +1618,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1621,7 +1638,7 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1641,7 +1658,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1661,7 +1678,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1681,7 +1698,7 @@
         <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1701,7 +1718,7 @@
         <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1721,7 +1738,7 @@
         <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1741,12 +1758,32 @@
         <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
       </c>
       <c r="F40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-06-25 08:12:10 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,26 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第610回</t>
+  </si>
+  <si>
+    <t>2025年6月25日（令和7年6月25日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１部会・小委員会に属する委員の指名等について
+２保険医療材料専門部会からの報告について
+３薬価専門部会からの報告について
+４医療提供体制等について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第609回</t>
@@ -48,13 +68,6 @@
 ６最適使用推進ガイドラインについて(報告)
 ７公知申請とされた適応外薬の保険適用について
 ８薬価基準から削除する品目について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -961,7 +974,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1018,7 +1031,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -1029,16 +1042,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1058,7 +1071,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1078,7 +1091,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1098,7 +1111,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1118,7 +1131,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1138,7 +1151,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1158,7 +1171,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1178,7 +1191,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1198,7 +1211,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1218,7 +1231,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1238,7 +1251,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1258,7 +1271,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1278,7 +1291,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1298,7 +1311,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1318,7 +1331,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1338,7 +1351,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1358,7 +1371,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1378,7 +1391,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1398,7 +1411,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1418,7 +1431,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1438,7 +1451,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1458,7 +1471,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1478,7 +1491,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1498,7 +1511,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1518,7 +1531,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1538,7 +1551,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1558,7 +1571,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1578,7 +1591,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1598,7 +1611,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1618,7 +1631,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1638,7 +1651,7 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1658,7 +1671,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1678,7 +1691,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1698,7 +1711,7 @@
         <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1718,7 +1731,7 @@
         <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1738,7 +1751,7 @@
         <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1758,7 +1771,7 @@
         <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1778,12 +1791,32 @@
         <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
       </c>
       <c r="F41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-07-09 08:12:48 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="135">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,27 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第611回</t>
+  </si>
+  <si>
+    <t>2025年7月9日（令和7年7月9日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
+２医薬品の新規薬価収載について
+３ＤＰＣにおける高額な新規の医薬品等への対応について
+４診療報酬改定結果検証部会からの報告について
+５ＤＰＣ対象病院の退出に係る報告について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第610回</t>
@@ -44,13 +65,6 @@
 ２保険医療材料専門部会からの報告について
 ３薬価専門部会からの報告について
 ４医療提供体制等について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -68,6 +82,10 @@
 ６最適使用推進ガイドラインについて(報告)
 ７公知申請とされた適応外薬の保険適用について
 ８薬価基準から削除する品目について
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -86,10 +104,6 @@
 ７DPC における高額な新規の医薬品等への対応について
 ８在宅自己注射について
 ９令和７年度における DPC/PDPS の現況について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -974,7 +988,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1451,7 +1465,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1471,7 +1485,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1817,6 +1831,26 @@
         <v>10</v>
       </c>
       <c r="F42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-07-16 08:12:27 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="138">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第612回</t>
+  </si>
+  <si>
+    <t>2025年7月16日（令和7年7月16日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
+２歯科用貴金属価格の随時改定について
+３外来について（その１）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第611回</t>
@@ -45,13 +64,6 @@
 ３ＤＰＣにおける高額な新規の医薬品等への対応について
 ４診療報酬改定結果検証部会からの報告について
 ５ＤＰＣ対象病院の退出に係る報告について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -988,7 +1000,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1065,7 +1077,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1076,16 +1088,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1105,7 +1117,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1125,7 +1137,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1145,7 +1157,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1165,7 +1177,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1185,7 +1197,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1205,7 +1217,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1225,7 +1237,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1245,7 +1257,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1265,7 +1277,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1285,7 +1297,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1305,7 +1317,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1325,7 +1337,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1345,7 +1357,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1365,7 +1377,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1385,7 +1397,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1405,7 +1417,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1425,7 +1437,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1445,7 +1457,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1465,7 +1477,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1485,7 +1497,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1505,7 +1517,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1525,7 +1537,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1545,7 +1557,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1565,7 +1577,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1585,7 +1597,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1605,7 +1617,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1625,7 +1637,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1645,7 +1657,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1665,7 +1677,7 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1685,7 +1697,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1705,7 +1717,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1725,7 +1737,7 @@
         <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1745,7 +1757,7 @@
         <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1765,7 +1777,7 @@
         <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1785,7 +1797,7 @@
         <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1805,7 +1817,7 @@
         <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1825,7 +1837,7 @@
         <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1845,12 +1857,32 @@
         <v>134</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
       </c>
       <c r="F43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-07-23 08:13:17 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="141">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第613回</t>
+  </si>
+  <si>
+    <t>2025年7月23日（令和7年7月23日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１主な施設基準の届出状況等について
+２医療ＤＸ推進体制整備加算等の要件の見直しについて
+３入院について（その１）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第612回</t>
@@ -43,13 +62,6 @@
     <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
 ２歯科用貴金属価格の随時改定について
 ３外来について（その１）
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -1000,7 +1012,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1097,7 +1109,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1108,16 +1120,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1137,7 +1149,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1157,7 +1169,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1177,7 +1189,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1197,7 +1209,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1217,7 +1229,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1237,7 +1249,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1257,7 +1269,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1277,7 +1289,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1297,7 +1309,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1317,7 +1329,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1337,7 +1349,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1357,7 +1369,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1377,7 +1389,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1397,7 +1409,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1417,7 +1429,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1437,7 +1449,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1457,7 +1469,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1477,7 +1489,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1497,7 +1509,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1517,7 +1529,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1537,7 +1549,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1557,7 +1569,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1577,7 +1589,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1597,7 +1609,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1617,7 +1629,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1637,7 +1649,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1657,7 +1669,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1677,7 +1689,7 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1697,7 +1709,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1717,7 +1729,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1737,7 +1749,7 @@
         <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1757,7 +1769,7 @@
         <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1777,7 +1789,7 @@
         <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1797,7 +1809,7 @@
         <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1817,7 +1829,7 @@
         <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1837,7 +1849,7 @@
         <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1857,7 +1869,7 @@
         <v>134</v>
       </c>
       <c r="D43" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1877,12 +1889,32 @@
         <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
       </c>
       <c r="F44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-08-06 08:02:27 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="144">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,30 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第614回</t>
+  </si>
+  <si>
+    <t>2025年8月6日（令和7年8月6日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１入院・外来医療等の調査・評価分科会からの報告について
+２医薬品の新規薬価収載について
+３医療機器及び臨床検査の保険適用について
+４ＤＰＣにおける高額な新規の医薬品等への対応について
+５保険医が投与することができる注射薬について
+６令和８年度診療報酬改定におけるＤＰＣ制度への参加又はＤＰＣ制度からの退出に係る届出の受付期間について
+７費用対効果評価の結果を踏まえた薬価の見直しについて
+８高額医薬品（認知症薬）に対する対応について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第613回</t>
@@ -43,13 +67,6 @@
     <t xml:space="preserve">１主な施設基準の届出状況等について
 ２医療ＤＸ推進体制整備加算等の要件の見直しについて
 ３入院について（その１）
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -89,6 +106,10 @@
 ２保険医療材料専門部会からの報告について
 ３薬価専門部会からの報告について
 ４医療提供体制等について
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -106,10 +127,6 @@
 ６最適使用推進ガイドラインについて(報告)
 ７公知申請とされた適応外薬の保険適用について
 ８薬価基準から削除する品目について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -1012,7 +1029,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1549,7 +1566,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1569,7 +1586,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1915,6 +1932,26 @@
         <v>10</v>
       </c>
       <c r="F45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-08-27 08:02:17 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="147">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,28 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第615回</t>
+  </si>
+  <si>
+    <t>2025年8月27日（令和7年8月27日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１再生医療等製品の医療保険上の取扱いについて
+２在宅について（その１）
+３医療機関等を取り巻く状況について
+４マイナ保険証の利用促進等について
+５スマートフォンでのマイナ保険証の利用開始に伴う資格確認方法の所要の見直しについて（諮問）
+６個別改定項目について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第614回</t>
@@ -51,13 +73,6 @@
 </t>
   </si>
   <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
-</t>
-  </si>
-  <si>
     <t>第613回</t>
   </si>
   <si>
@@ -79,6 +94,10 @@
     <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
 ２歯科用貴金属価格の随時改定について
 ３外来について（その１）
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -106,10 +125,6 @@
 ２保険医療材料専門部会からの報告について
 ３薬価専門部会からの報告について
 ４医療提供体制等について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -1029,7 +1044,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1126,7 +1141,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1137,16 +1152,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1166,7 +1181,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1186,7 +1201,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1206,7 +1221,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1226,7 +1241,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1246,7 +1261,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1266,7 +1281,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1286,7 +1301,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1306,7 +1321,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1326,7 +1341,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1346,7 +1361,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1366,7 +1381,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1386,7 +1401,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1406,7 +1421,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1426,7 +1441,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1446,7 +1461,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1466,7 +1481,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1486,7 +1501,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1506,7 +1521,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1526,7 +1541,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1546,7 +1561,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1566,7 +1581,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1586,7 +1601,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1606,7 +1621,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1626,7 +1641,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1646,7 +1661,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1666,7 +1681,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1686,7 +1701,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1706,7 +1721,7 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1726,7 +1741,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1746,7 +1761,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1766,7 +1781,7 @@
         <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1786,7 +1801,7 @@
         <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1806,7 +1821,7 @@
         <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1826,7 +1841,7 @@
         <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1846,7 +1861,7 @@
         <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1866,7 +1881,7 @@
         <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1886,7 +1901,7 @@
         <v>134</v>
       </c>
       <c r="D43" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1906,7 +1921,7 @@
         <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -1926,7 +1941,7 @@
         <v>140</v>
       </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -1946,12 +1961,32 @@
         <v>143</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
       </c>
       <c r="F46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" t="s">
+        <v>146</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-09-10 08:02:25 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="150">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第616回</t>
+  </si>
+  <si>
+    <t>2025年9月10日（令和7年9月10日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１歯科医療について（その１）
+２調剤について（その１）
+３費用対効果評価専門組織からの報告について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第615回</t>
@@ -46,13 +65,7 @@
 ４マイナ保険証の利用促進等について
 ５スマートフォンでのマイナ保険証の利用開始に伴う資格確認方法の所要の見直しについて（諮問）
 ６個別改定項目について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
+７答申について
 </t>
   </si>
   <si>
@@ -85,6 +98,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">議事録
+</t>
+  </si>
+  <si>
     <t>第612回</t>
   </si>
   <si>
@@ -94,10 +111,6 @@
     <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
 ２歯科用貴金属価格の随時改定について
 ３外来について（その１）
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -1044,7 +1057,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1621,7 +1634,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1641,7 +1654,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1987,6 +2000,26 @@
         <v>10</v>
       </c>
       <c r="F47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-09-17 08:02:14 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="153">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,30 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第617回</t>
+  </si>
+  <si>
+    <t>2025年9月17日（令和7年9月17日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１部会・小委員会に属する委員の指名等について
+２最近の医療費の動向について
+３医療機器の保険適用について　
+４最適使用推進ガイドラインについて（報告）
+５公知申請とされた適応外薬の保険適用について　
+６薬価基準から削除する品目について
+７令和６年能登半島地震に伴う被災地特例措置について
+８選定療養等の募集結果の報告について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第616回</t>
@@ -43,13 +67,6 @@
     <t xml:space="preserve">１歯科医療について（その１）
 ２調剤について（その１）
 ３費用対効果評価専門組織からの報告について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -1057,7 +1074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1154,7 +1171,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1165,16 +1182,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1194,7 +1211,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1214,7 +1231,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1234,7 +1251,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1254,7 +1271,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1274,7 +1291,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1294,7 +1311,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1314,7 +1331,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1334,7 +1351,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1354,7 +1371,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1374,7 +1391,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1394,7 +1411,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1414,7 +1431,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1434,7 +1451,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1454,7 +1471,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1474,7 +1491,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1494,7 +1511,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1514,7 +1531,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1534,7 +1551,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1554,7 +1571,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1574,7 +1591,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1594,7 +1611,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1614,7 +1631,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1634,7 +1651,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1654,7 +1671,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1674,7 +1691,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1694,7 +1711,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1714,7 +1731,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1734,7 +1751,7 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1754,7 +1771,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1774,7 +1791,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1794,7 +1811,7 @@
         <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1814,7 +1831,7 @@
         <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1834,7 +1851,7 @@
         <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1854,7 +1871,7 @@
         <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1874,7 +1891,7 @@
         <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1894,7 +1911,7 @@
         <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1914,7 +1931,7 @@
         <v>134</v>
       </c>
       <c r="D43" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1934,7 +1951,7 @@
         <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -1954,7 +1971,7 @@
         <v>140</v>
       </c>
       <c r="D45" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -1974,7 +1991,7 @@
         <v>143</v>
       </c>
       <c r="D46" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
@@ -1994,7 +2011,7 @@
         <v>146</v>
       </c>
       <c r="D47" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -2014,12 +2031,32 @@
         <v>149</v>
       </c>
       <c r="D48" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
       </c>
       <c r="F48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-10-01 08:02:22 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="156">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第618回</t>
+  </si>
+  <si>
+    <t>2025年10月1日（令和7年10月1日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１入院・外来医療等の調査・評価分科会からの報告について
+２在宅について（その２）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第617回</t>
@@ -48,13 +66,6 @@
 ６薬価基準から削除する品目について
 ７令和６年能登半島地震に伴う被災地特例措置について
 ８選定療養等の募集結果の報告について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -1074,7 +1085,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1191,7 +1202,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1202,16 +1213,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1231,7 +1242,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1251,7 +1262,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1271,7 +1282,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1291,7 +1302,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1311,7 +1322,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1331,7 +1342,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1351,7 +1362,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1371,7 +1382,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1391,7 +1402,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1411,7 +1422,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1431,7 +1442,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1451,7 +1462,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1471,7 +1482,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1491,7 +1502,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1511,7 +1522,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1531,7 +1542,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1551,7 +1562,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1571,7 +1582,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1591,7 +1602,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1611,7 +1622,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1631,7 +1642,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1651,7 +1662,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1671,7 +1682,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1691,7 +1702,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1711,7 +1722,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1731,7 +1742,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1751,7 +1762,7 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1771,7 +1782,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1791,7 +1802,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1811,7 +1822,7 @@
         <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1831,7 +1842,7 @@
         <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1851,7 +1862,7 @@
         <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1871,7 +1882,7 @@
         <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1891,7 +1902,7 @@
         <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1911,7 +1922,7 @@
         <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1931,7 +1942,7 @@
         <v>134</v>
       </c>
       <c r="D43" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1951,7 +1962,7 @@
         <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -1971,7 +1982,7 @@
         <v>140</v>
       </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -1991,7 +2002,7 @@
         <v>143</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
@@ -2011,7 +2022,7 @@
         <v>146</v>
       </c>
       <c r="D47" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -2031,7 +2042,7 @@
         <v>149</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
@@ -2051,12 +2062,32 @@
         <v>152</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
       </c>
       <c r="F49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-10-08 08:02:18 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="159">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第619回</t>
+  </si>
+  <si>
+    <t>2025年10月8日（令和7年10月8日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１再生医療等製品の医療保険上の取扱いについて
+２診療報酬調査専門組織「医療機関等における消費税負担に関する分科会」からの報告について
+３入院について（その２）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第618回</t>
@@ -42,13 +61,6 @@
   <si>
     <t xml:space="preserve">１入院・外来医療等の調査・評価分科会からの報告について
 ２在宅について（その２）
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -1085,7 +1097,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1222,7 +1234,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1233,16 +1245,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1262,7 +1274,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1282,7 +1294,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -1302,7 +1314,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1322,7 +1334,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1342,7 +1354,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1362,7 +1374,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1382,7 +1394,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1402,7 +1414,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1422,7 +1434,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1442,7 +1454,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1462,7 +1474,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1482,7 +1494,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1502,7 +1514,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1522,7 +1534,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1542,7 +1554,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1562,7 +1574,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1582,7 +1594,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1602,7 +1614,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1622,7 +1634,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1642,7 +1654,7 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1662,7 +1674,7 @@
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1682,7 +1694,7 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1702,7 +1714,7 @@
         <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1722,7 +1734,7 @@
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1742,7 +1754,7 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1762,7 +1774,7 @@
         <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1782,7 +1794,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1802,7 +1814,7 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1822,7 +1834,7 @@
         <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1842,7 +1854,7 @@
         <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1862,7 +1874,7 @@
         <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1882,7 +1894,7 @@
         <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1902,7 +1914,7 @@
         <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1922,7 +1934,7 @@
         <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1942,7 +1954,7 @@
         <v>134</v>
       </c>
       <c r="D43" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1962,7 +1974,7 @@
         <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -1982,7 +1994,7 @@
         <v>140</v>
       </c>
       <c r="D45" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -2002,7 +2014,7 @@
         <v>143</v>
       </c>
       <c r="D46" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
@@ -2022,7 +2034,7 @@
         <v>146</v>
       </c>
       <c r="D47" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -2042,7 +2054,7 @@
         <v>149</v>
       </c>
       <c r="D48" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
@@ -2062,7 +2074,7 @@
         <v>152</v>
       </c>
       <c r="D49" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
@@ -2082,12 +2094,32 @@
         <v>155</v>
       </c>
       <c r="D50" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
       </c>
       <c r="F50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-10-17 08:02:18 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第621回</t>
+  </si>
+  <si>
+    <t>2025年10月17日（令和7年10月17日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１外来について（その２）
+２個別事項について（後発医薬品・バイオ後続品の使用体制、服用薬剤調整支援等の評価）
+３歯科用貴金属価格の随時改定について　
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第620回</t>
@@ -49,13 +68,6 @@
 ７ＤＰＣにおける高額な新規の医薬品等への対応について　　
 ８在宅自己注射について　　
 ９ＤＰＣ対象病院の退出に係る報告について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
 </sst>
@@ -388,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -434,6 +446,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update num.txt | 2025-10-24 08:02:25 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>回数</t>
   </si>
@@ -34,6 +34,24 @@
     <t>開催案内</t>
   </si>
   <si>
+    <t>第622回</t>
+  </si>
+  <si>
+    <t>2025年10月24日（令和7年10月24日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１個別事項について（その２）精神医療①
+２個別事項について（その３）（敷地内薬局）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
+  </si>
+  <si>
     <t>第621回</t>
   </si>
   <si>
@@ -41,15 +59,8 @@
   </si>
   <si>
     <t xml:space="preserve">１外来について（その２）
-２個別事項について（後発医薬品・バイオ後続品の使用体制、服用薬剤調整支援等の評価）
+２個別事項について（その１）後発医薬品・バイオ後続品の使用体制、服用薬剤調整支援等の評価
 ３歯科用貴金属価格の随時改定について　
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -400,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -466,6 +477,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update num.txt | 2025-10-29 08:02:29 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,26 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第623回</t>
+  </si>
+  <si>
+    <t>2025年10月29日（令和7年10月29日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１薬価基準から削除する品目について
+２入院について（その３）　
+３個別事項について（その４）移植医療
+４医療機関を取り巻く状況について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第622回</t>
@@ -42,13 +62,6 @@
   <si>
     <t xml:space="preserve">１個別事項について（その２）精神医療①
 ２個別事項について（その３）（敷地内薬局）
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -411,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -497,6 +510,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update num.txt | 2025-11-05 08:02:21 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,30 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第624回</t>
+  </si>
+  <si>
+    <t>2025年11月5日（令和7年11月5日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１部会・小委員会に属する委員の指名等について
+２医薬品の新規薬価収載等について
+３最適使用推進ガイドラインについて
+４費用対効果評価の結果を踏まえた薬価の見直しについて　　
+５ＰＥＴの保険適用について　　
+６ＤＰＣにおける高額な新規の医薬品等への対応について　　
+７入院について（その４）　　
+８個別事項について（その５）がん対策・難病対策・透析医療・緩和ケア
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第623回</t>
@@ -44,13 +68,6 @@
 ２入院について（その３）　
 ３個別事項について（その４）移植医療
 ４医療機関を取り巻く状況について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -424,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -530,6 +547,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update num.txt | 2025-11-07 08:02:23 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第625回</t>
+  </si>
+  <si>
+    <t>2025年11月7日（令和7年11月7日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１外来について（その３）
+２入院時の食費・光熱水費について（その１）
+３個別事項について（その６）入院から外来への移行
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第624回</t>
@@ -48,13 +67,6 @@
 ６ＤＰＣにおける高額な新規の医薬品等への対応について　　
 ７入院について（その４）　　
 ８個別事項について（その５）がん対策・難病対策・透析医療・緩和ケア
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -441,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -567,6 +579,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update num.txt | 2025-11-12 08:02:23 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第626回</t>
+  </si>
+  <si>
+    <t>2025年11月12日（令和7年11月12日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
+２在宅について（その３）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第625回</t>
@@ -43,13 +61,6 @@
     <t xml:space="preserve">１外来について（その３）
 ２入院時の食費・光熱水費について（その１）
 ３個別事項について（その６）入院から外来への移行
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -453,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -599,6 +610,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update num.txt | 2025-11-14 08:02:21 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,26 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第627回</t>
+  </si>
+  <si>
+    <t>2025年11月14日（令和7年11月14日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
+２入院について（その５）
+３在宅について（その４）
+４個別事項について（その７）長期収載品の選定療養①
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第626回</t>
@@ -42,13 +62,6 @@
   <si>
     <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
 ２在宅について（その３）
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -464,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -630,6 +643,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update num.txt | 2025-11-19 08:02:19 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第628回</t>
+  </si>
+  <si>
+    <t>2025年11月19日（令和7年11月19日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１入院について（その６）
+２個別事項について（その８）小児・周産期医療、感染症対策、医療安全、災害医療
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第627回</t>
@@ -44,13 +62,6 @@
 ２入院について（その５）
 ３在宅について（その４）
 ４個別事項について（その７）長期収載品の選定療養①
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -145,6 +156,10 @@
 ７ＤＰＣにおける高額な新規の医薬品等への対応について　　
 ８在宅自己注射について　　
 ９ＤＰＣ対象病院の退出に係る報告について
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
 </sst>
@@ -477,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -663,6 +678,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update num.txt | 2025-11-21 08:02:22 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第629回</t>
+  </si>
+  <si>
+    <t>2025年11月21日（令和7年11月21日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１診療報酬改定結果検証部会からの報告について
+２歯科医療について（その２）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第628回</t>
@@ -42,13 +60,6 @@
   <si>
     <t xml:space="preserve">１入院について（その６）
 ２個別事項について（その８）小児・周産期医療、感染症対策、医療安全、災害医療
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -126,6 +137,10 @@
   <si>
     <t xml:space="preserve">１個別事項について（その２）精神医療①
 ２個別事項について（その３）（敷地内薬局）
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -156,10 +171,6 @@
 ７ＤＰＣにおける高額な新規の医薬品等への対応について　　
 ８在宅自己注射について　　
 ９ＤＰＣ対象病院の退出に係る報告について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
 </sst>
@@ -492,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -669,7 +680,7 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -680,21 +691,41 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-11-26 08:02:27 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第630回</t>
+  </si>
+  <si>
+    <t>2025年11月26日（令和7年11月26日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１調査実施小委員会からの報告について
+２入院について（その７）
+３個別事項について（その９）データ提出加算
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第629回</t>
@@ -42,13 +61,6 @@
   <si>
     <t xml:space="preserve">１診療報酬改定結果検証部会からの報告について
 ２歯科医療について（その２）
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -503,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -680,7 +692,7 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -691,16 +703,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -720,12 +732,32 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
       </c>
       <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-11-28 08:02:19 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第631回</t>
+  </si>
+  <si>
+    <t>2025年11月28日（令和7年11月28日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１診療報酬調査専門組織「医療機関等における消費税負担に関する分科会」からの報告について
+２調剤について（その２）
+３個別事項について（その１０）人口・医療資源の少ない地域、救急医療、業務の簡素化
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第630回</t>
@@ -43,13 +62,6 @@
     <t xml:space="preserve">１調査実施小委員会からの報告について
 ２入院について（その７）
 ３個別事項について（その９）データ提出加算
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -141,6 +153,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">議事録
+</t>
+  </si>
+  <si>
     <t>第622回</t>
   </si>
   <si>
@@ -149,10 +165,6 @@
   <si>
     <t xml:space="preserve">１個別事項について（その２）精神医療①
 ２個別事項について（その３）（敷地内薬局）
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -515,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -761,6 +773,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update num.txt | 2025-12-03 08:02:22 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,28 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第632回</t>
+  </si>
+  <si>
+    <t>2025年12月3日（令和7年12月3日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１※議題１は開催直前に掲載いたします。
+２医療技術評価分科会からの報告
+３個別事項その１１（届出や算定方法の明確化）
+４入院時の食費・光熱水費について（その２）
+５医療経済実態調査の結果に対する見解について
+６その他
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第631回</t>
@@ -43,13 +65,6 @@
     <t xml:space="preserve">１診療報酬調査専門組織「医療機関等における消費税負担に関する分科会」からの報告について
 ２調剤について（その２）
 ３個別事項について（その１０）人口・医療資源の少ない地域、救急医療、業務の簡素化
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -527,7 +542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -724,7 +739,7 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -735,16 +750,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -764,7 +779,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -784,12 +799,32 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
       </c>
       <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-12-05 08:02:20 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t>回数</t>
   </si>
@@ -34,25 +34,38 @@
     <t>開催案内</t>
   </si>
   <si>
+    <t>第633回</t>
+  </si>
+  <si>
+    <t>2025年12月5日（令和7年12月5日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１個別事項について（その１２）後発医薬品・バイオ後続品の使用体制②
+２個別事項について（その１３）精神医療②
+３個別事項について（その１４）技術的事項
+４賃上げについて（その１）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
+  </si>
+  <si>
     <t>第632回</t>
   </si>
   <si>
     <t>2025年12月3日（令和7年12月3日）</t>
   </si>
   <si>
-    <t xml:space="preserve">１※議題１は開催直前に掲載いたします。
+    <t xml:space="preserve">１薬価調査、特定保険医療材料価格調査の結果速報について
 ２医療技術評価分科会からの報告
 ３個別事項その１１（届出や算定方法の明確化）
 ４入院時の食費・光熱水費について（その２）
 ５医療経済実態調査の結果に対する見解について
 ６その他
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -542,7 +555,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -759,7 +772,7 @@
         <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -770,16 +783,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>41</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -799,7 +812,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -819,12 +832,32 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
       </c>
       <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-12-10 08:02:24 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第634回</t>
+  </si>
+  <si>
+    <t>2025年12月10日（令和7年12月10日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１費用対効果評価専門組織からの報告について
+２令和７年度補正予算案の閣議決定について
+３令和８年度診療報酬改定に関する基本的な見解（各号意見）について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第633回</t>
@@ -44,13 +63,6 @@
 ２個別事項について（その１３）精神医療②
 ３個別事項について（その１４）技術的事項
 ４賃上げについて（その１）
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -555,7 +567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -792,7 +804,7 @@
         <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -803,16 +815,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -832,7 +844,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -852,12 +864,32 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
       <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-12-12 08:02:34 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,26 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第635回</t>
+  </si>
+  <si>
+    <t>2025年12月12日（令和7年12月12日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１「令和８年度診療報酬改定の基本方針」について
+２個別事項について（その１５）医薬品その他
+３入院について（その８）
+４令和８年度診療報酬改定への意見について（公益委員案の提示）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第634回</t>
@@ -43,13 +63,6 @@
     <t xml:space="preserve">１費用対効果評価専門組織からの報告について
 ２令和７年度補正予算案の閣議決定について
 ３令和８年度診療報酬改定に関する基本的な見解（各号意見）について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -567,7 +580,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -824,7 +837,7 @@
         <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -835,16 +848,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>47</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -864,7 +877,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -884,12 +897,32 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
       </c>
       <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-12-17 08:02:20 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t>2025年12月17日（令和7年12月17日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１医療機器の保険適用について
+２先進医療会議からの報告について
+３最適使用推進ガイドラインについて(報告) 
+４公知申請とされた適応外薬の保険適用について
+５ＤＰＣ/ＰＤＰＳにおける令和６年 10 月から令和７年９月までの間の豪雨及び暴風雨による災害を踏まえた対応について
+６個別事項について（その１６）長期収載品の選定療養➁
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第635回</t>
@@ -44,13 +63,6 @@
 ２個別事項について（その１５）医薬品その他
 ３入院について（その８）
 ４令和８年度診療報酬改定への意見について（公益委員案の提示）
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -193,6 +205,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">議事録
+</t>
+  </si>
+  <si>
     <t>第623回</t>
   </si>
   <si>
@@ -203,10 +219,6 @@
 ２入院について（その３）　
 ３個別事項について（その４）移植医療
 ４医療機関を取り巻く状況について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -580,7 +592,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -617,313 +629,333 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>46</v>
       </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
         <v>48</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>49</v>
       </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
         <v>51</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>52</v>
       </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
         <v>56</v>
       </c>
-      <c r="D17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" t="s">
-        <v>9</v>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update num.txt | 2025-12-19 08:02:27 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
   <si>
     <t>回数</t>
   </si>
@@ -34,7 +34,26 @@
     <t>開催案内</t>
   </si>
   <si>
+    <t>第637回</t>
+  </si>
+  <si>
+    <t>2025年12月19日（令和7年12月19日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１個別事項について（その１７）これまでの御指摘に対する回答について
+２個別事項について（その１８）医療ＤＸ
+３個別事項について（その１９）残薬対策 
+</t>
+  </si>
+  <si>
     <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
+  </si>
+  <si>
+    <t>第636回</t>
   </si>
   <si>
     <t>2025年12月17日（令和7年12月17日）</t>
@@ -46,10 +65,6 @@
 ４公知申請とされた適応外薬の保険適用について
 ５ＤＰＣ/ＰＤＰＳにおける令和６年 10 月から令和７年９月までの間の豪雨及び暴風雨による災害を踏まえた対応について
 ６個別事項について（その１６）長期収載品の選定療養➁
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -592,7 +607,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -629,253 +644,253 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -889,73 +904,93 @@
         <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update num.txt | 2025-12-24 08:02:20 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,24 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第638回</t>
+  </si>
+  <si>
+    <t>2025年12月24日（令和7年12月24日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１個別事項について（その２０）技術的事項（その２）・これまでの御指摘に対する回答
+２医療法等改正を踏まえた対応について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第637回</t>
@@ -43,13 +61,6 @@
     <t xml:space="preserve">１個別事項について（その１７）これまでの御指摘に対する回答について
 ２個別事項について（その１８）医療ＤＸ
 ３個別事項について（その１９）残薬対策 
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -103,6 +114,10 @@
 ２個別事項について（その１３）精神医療②
 ３個別事項について（その１４）技術的事項
 ４賃上げについて（その１）
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -217,10 +232,6 @@
 ６ＤＰＣにおける高額な新規の医薬品等への対応について　　
 ７入院について（その４）　　
 ８個別事項について（その５）がん対策・難病対策・透析医療・緩和ケア
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -607,7 +618,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -744,7 +755,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -755,16 +766,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -775,16 +786,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -795,16 +806,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -815,16 +826,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -835,16 +846,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -855,16 +866,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -875,16 +886,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -895,16 +906,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -924,7 +935,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -944,7 +955,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -964,7 +975,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -984,12 +995,32 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
       <c r="F19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2025-12-26 08:02:20 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,28 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第639回</t>
+  </si>
+  <si>
+    <t>2025年12月26日（令和7年12月26日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１令和８年度診療報酬改定の改定率等について
+２令和８年度費用対効果評価制度改革の骨子（案）について
+３令和８年度保険医療材料制度改革の骨子（案）について
+４令和８年度薬価制度改革の骨子（案）について
+５令和８年度診療報酬改定への意見について（各号意見）
+６その他
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第638回</t>
@@ -42,13 +64,6 @@
   <si>
     <t xml:space="preserve">１個別事項について（その２０）技術的事項（その２）・これまでの御指摘に対する回答
 ２医療法等改正を踏まえた対応について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -618,7 +633,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -755,7 +770,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -766,16 +781,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -795,7 +810,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -815,7 +830,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -835,7 +850,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -855,7 +870,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -875,7 +890,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -895,7 +910,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -915,7 +930,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -935,7 +950,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -955,7 +970,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -975,7 +990,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -995,7 +1010,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1015,12 +1030,32 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
       </c>
       <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2026-01-09 08:02:29 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,26 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第640回</t>
+  </si>
+  <si>
+    <t>2026年1月9日（令和8年1月9日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１物価対応について（その１）
+２選定療養等募集を受けた対応について
+３個別事項について（その２１）近視進行抑制薬の処方に係る検査について
+４これまでの議論の整理（案）について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第639回</t>
@@ -49,13 +69,6 @@
 </t>
   </si>
   <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
-</t>
-  </si>
-  <si>
     <t>第638回</t>
   </si>
   <si>
@@ -107,6 +120,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">議事録
+</t>
+  </si>
+  <si>
     <t>第634回</t>
   </si>
   <si>
@@ -129,10 +146,6 @@
 ２個別事項について（その１３）精神医療②
 ３個別事項について（その１４）技術的事項
 ４賃上げについて（その１）
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -633,7 +646,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -770,7 +783,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -781,16 +794,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -810,7 +823,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -830,7 +843,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -850,7 +863,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -870,7 +883,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -890,7 +903,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -910,7 +923,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -930,7 +943,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -950,7 +963,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -970,7 +983,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -990,7 +1003,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1010,7 +1023,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1030,7 +1043,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1050,12 +1063,32 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
       </c>
       <c r="F21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2026-01-14 08:02:28 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,33 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第641回</t>
+  </si>
+  <si>
+    <t>2026年1月14日（令和8年1月14日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１先進医療会議及び患者申出療養評価会議からの報告について
+２医療法等改正に伴う療養担当規則等の所要の見直しについて（諮問）
+３医療法等改正を踏まえた対応について（その２）
+４入院について（その９）
+５賃上げについて（その２）
+６物価対応について（その２）
+７これまでの議論の整理（案）について
+８令和８年度診療報酬改定について（諮問）
+９再生医療等製品の医療保険上の取扱いについて
+10費用対効果評価専門部会・薬価専門部会・保険医療材料専門部会 合同部会からの報告について
+11その他
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第640回</t>
@@ -44,13 +71,6 @@
 ２選定療養等募集を受けた対応について
 ３個別事項について（その２１）近視進行抑制薬の処方に係る検査について
 ４これまでの議論の整理（案）について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -646,7 +666,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -783,7 +803,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -794,16 +814,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -823,7 +843,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -843,7 +863,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -863,7 +883,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -883,7 +903,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -903,7 +923,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -923,7 +943,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -943,7 +963,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -963,7 +983,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -983,7 +1003,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1003,7 +1023,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1023,7 +1043,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1043,7 +1063,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1063,7 +1083,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1083,12 +1103,32 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
       </c>
       <c r="F22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2026-01-16 08:02:29 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="78">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,29 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第642回</t>
+  </si>
+  <si>
+    <t>2026年1月16日（令和8年1月16日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１令和８年度費用対効果評価制度の見直しについて
+２令和８年度保険医療材料制度の見直しについて
+３令和８年度薬価制度の見直しについて
+４市場拡大再算定について
+５歯科用貴金属価格の随時改定について
+６個別改定項目について（医療法等改正に伴う療養担当規則等の所要の見直しについて）
+７医療技術評価分科会からの報告について
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第641回</t>
@@ -54,13 +77,6 @@
 </t>
   </si>
   <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
-</t>
-  </si>
-  <si>
     <t>第640回</t>
   </si>
   <si>
@@ -112,6 +128,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">議事録
+</t>
+  </si>
+  <si>
     <t>第636回</t>
   </si>
   <si>
@@ -137,10 +157,6 @@
 ２個別事項について（その１５）医薬品その他
 ３入院について（その８）
 ４令和８年度診療報酬改定への意見について（公益委員案の提示）
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -666,7 +682,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -803,7 +819,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -814,16 +830,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -843,7 +859,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -863,7 +879,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -883,7 +899,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -903,7 +919,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -923,7 +939,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -943,7 +959,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -963,7 +979,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -983,7 +999,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1003,7 +1019,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1023,7 +1039,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1043,7 +1059,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1063,7 +1079,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1083,7 +1099,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1103,7 +1119,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1123,12 +1139,32 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
       </c>
       <c r="F23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2026-01-21 08:02:38 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,21 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t>2026年1月21日（令和8年1月21日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１令和８年度診療報酬改定に係る検討状況について
+２意見発表者による意見発表、中医協委員からの質問
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第642回</t>
@@ -46,14 +61,8 @@
 ４市場拡大再算定について
 ５歯科用貴金属価格の随時改定について
 ６個別改定項目について（医療法等改正に伴う療養担当規則等の所要の見直しについて）
-７医療技術評価分科会からの報告について
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
+７答申について（医療法等改正に伴う療養担当規則等の所要の見直しについて）
+８医療技術評価分科会からの報告について
 </t>
   </si>
   <si>
@@ -682,7 +691,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -719,453 +728,473 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
         <v>48</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>49</v>
       </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
         <v>51</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>52</v>
       </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="s">
-        <v>56</v>
-      </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
         <v>57</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>58</v>
       </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
         <v>60</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>61</v>
       </c>
-      <c r="C19" t="s">
-        <v>62</v>
-      </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
         <v>63</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>64</v>
       </c>
-      <c r="C20" t="s">
-        <v>65</v>
-      </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
         <v>66</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>67</v>
       </c>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>70</v>
       </c>
-      <c r="C22" t="s">
-        <v>71</v>
-      </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
         <v>72</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>73</v>
       </c>
-      <c r="C23" t="s">
-        <v>74</v>
-      </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
         <v>75</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>76</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
         <v>77</v>
       </c>
-      <c r="D24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
-        <v>9</v>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update num.txt | 2026-01-23 08:02:42 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="84">
   <si>
     <t>回数</t>
   </si>
@@ -34,7 +34,25 @@
     <t>開催案内</t>
   </si>
   <si>
+    <t>第644回</t>
+  </si>
+  <si>
+    <t>2026年1月23日（令和8年1月23日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
+２個別改定項目について（その１）
+</t>
+  </si>
+  <si>
     <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
+  </si>
+  <si>
+    <t>第643回</t>
   </si>
   <si>
     <t>2026年1月21日（令和8年1月21日）</t>
@@ -42,10 +60,6 @@
   <si>
     <t xml:space="preserve">１令和８年度診療報酬改定に係る検討状況について
 ２意見発表者による意見発表、中医協委員からの質問
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -691,7 +705,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -728,133 +742,133 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -868,333 +882,353 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update num.txt | 2026-01-28 08:02:33 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,25 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第645回</t>
+  </si>
+  <si>
+    <t>2026年1月28日（令和8年1月28日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１特定保険医療材料の機能区分の見直し等について
+２個別改定項目について（その２）
+３答申書の附帯意見案について（その１）
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第644回</t>
@@ -42,13 +61,6 @@
   <si>
     <t xml:space="preserve">１医療機器及び臨床検査の保険適用について
 ２個別改定項目について（その１）
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -128,6 +140,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">議事録
+</t>
+  </si>
+  <si>
     <t>第638回</t>
   </si>
   <si>
@@ -148,10 +164,6 @@
     <t xml:space="preserve">１個別事項について（その１７）これまでの御指摘に対する回答について
 ２個別事項について（その１８）医療ＤＸ
 ３個別事項について（その１９）残薬対策 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -705,7 +717,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -862,7 +874,7 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -873,16 +885,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -902,7 +914,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -922,7 +934,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -942,7 +954,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -962,7 +974,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -982,7 +994,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1002,7 +1014,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1022,7 +1034,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1042,7 +1054,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1062,7 +1074,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1082,7 +1094,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1102,7 +1114,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1122,7 +1134,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1142,7 +1154,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1162,7 +1174,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1182,7 +1194,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1202,7 +1214,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1222,12 +1234,32 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
       </c>
       <c r="F26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2026-01-30 08:05:07 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,27 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第646回</t>
+  </si>
+  <si>
+    <t>2026年1月30日（令和8年1月30日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１バイオ後続品等の最適使用推進ガイドラインの取扱いについて
+２パブリックコメント、公聴会の報告について
+３個別改定項目について（その３）
+３答申書の附帯意見案について（その２）
+３その他
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第645回</t>
@@ -43,13 +64,6 @@
     <t xml:space="preserve">１特定保険医療材料の機能区分の見直し等について
 ２個別改定項目について（その２）
 ３答申書の附帯意見案について（その１）
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
 </t>
   </si>
   <si>
@@ -89,6 +103,10 @@
 ６個別改定項目について（医療法等改正に伴う療養担当規則等の所要の見直しについて）
 ７答申について（医療法等改正に伴う療養担当規則等の所要の見直しについて）
 ８医療技術評価分科会からの報告について
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -137,10 +155,6 @@
 ４令和８年度薬価制度改革の骨子（案）について
 ５令和８年度診療報酬改定への意見について（各号意見）
 ６その他
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -717,7 +731,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -834,7 +848,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -845,16 +859,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -865,16 +879,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -894,7 +908,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -914,7 +928,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -934,7 +948,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -954,7 +968,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -974,7 +988,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -994,7 +1008,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1014,7 +1028,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1034,7 +1048,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1054,7 +1068,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1074,7 +1088,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1094,7 +1108,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1114,7 +1128,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1134,7 +1148,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1154,7 +1168,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1174,7 +1188,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1194,7 +1208,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1214,7 +1228,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1234,7 +1248,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1254,12 +1268,32 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
       </c>
       <c r="F27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update num.txt | 2026-02-13 08:05:36 JST
</commit_message>
<xml_diff>
--- a/docs/output.xlsx
+++ b/docs/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="93">
   <si>
     <t>回数</t>
   </si>
@@ -32,6 +32,23 @@
   </si>
   <si>
     <t>開催案内</t>
+  </si>
+  <si>
+    <t>第647回</t>
+  </si>
+  <si>
+    <t>2026年2月13日（令和8年2月13日）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">※ 掲載準備中_x000D_
+</t>
+  </si>
+  <si>
+    <t>－</t>
+  </si>
+  <si>
+    <t xml:space="preserve">資料
+</t>
   </si>
   <si>
     <t>第646回</t>
@@ -43,15 +60,12 @@
     <t xml:space="preserve">１バイオ後続品等の最適使用推進ガイドラインの取扱いについて
 ２パブリックコメント、公聴会の報告について
 ３個別改定項目について（その３）
-３答申書の附帯意見案について（その２）
-３その他
-</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t xml:space="preserve">資料
+４答申書の附帯意見案について（その２）
+５その他
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -103,10 +117,6 @@
 ６個別改定項目について（医療法等改正に伴う療養担当規則等の所要の見直しについて）
 ７答申について（医療法等改正に伴う療養担当規則等の所要の見直しについて）
 ８医療技術評価分科会からの報告について
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">議事録
 </t>
   </si>
   <si>
@@ -731,7 +741,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -788,7 +798,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -799,16 +809,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -819,16 +829,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -839,16 +849,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -868,7 +878,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -888,7 +898,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -908,7 +918,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -928,7 +938,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -948,7 +958,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -968,7 +978,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -988,7 +998,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1008,7 +1018,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1028,7 +1038,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1048,7 +1058,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1068,7 +1078,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1088,7 +1098,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1108,7 +1118,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1128,7 +1138,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1148,7 +1158,7 @@
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1168,7 +1178,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1188,7 +1198,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1208,7 +1218,7 @@
         <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1228,7 +1238,7 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1248,7 +1258,7 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1268,7 +1278,7 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1288,12 +1298,32 @@
         <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
       </c>
       <c r="F28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>